<commit_message>
Fixes to various issues that have came up
</commit_message>
<xml_diff>
--- a/core-boards/diagnostics-main/Parts List.xlsx
+++ b/core-boards/diagnostics-main/Parts List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drwar\OneDrive\Documents\GitHub\igvc-electrical\core-boards\diagnostics-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drwar\Desktop\IGVC\igvc-electrical\core-boards\diagnostics-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{90B91A56-3370-400E-8106-8702C9321A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7353C8C1-E9A2-4134-8146-43EEF9F9F5F4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C4AA1-540B-4C9E-B593-018B6BA187A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21816" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Part</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t xml:space="preserve">	900-0022232021-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/MCP2515T-I-ST/MCP2515T-I-STCT-ND/4307903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	MCP2515T-I/STCT-ND</t>
+  </si>
+  <si>
+    <t>Can Controller</t>
   </si>
 </sst>
 </file>
@@ -600,15 +609,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -638,7 +651,7 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -665,7 +678,7 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -692,7 +705,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>45</v>
       </c>
@@ -719,7 +732,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>44</v>
       </c>
@@ -746,7 +759,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -773,7 +786,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>42</v>
       </c>
@@ -800,7 +813,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -827,7 +840,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -854,7 +867,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>38</v>
       </c>
@@ -881,7 +894,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
@@ -908,7 +921,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
@@ -935,7 +948,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
@@ -964,7 +977,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -993,7 +1006,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>47</v>
       </c>
@@ -1020,21 +1033,21 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16">
         <v>1</v>
       </c>
@@ -1047,21 +1060,21 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="H17" s="6"/>
       <c r="I17">
         <v>1</v>
       </c>
@@ -1072,23 +1085,23 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18">
         <v>1</v>
       </c>
@@ -1101,21 +1114,21 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="H19" s="6"/>
       <c r="I19">
         <v>1</v>
       </c>
@@ -1125,24 +1138,24 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="P19" s="4"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="H20" s="5"/>
       <c r="I20">
         <v>1</v>
       </c>
@@ -1155,83 +1168,95 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="H22" s="6"/>
       <c r="I22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="6" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1244,74 +1269,79 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="6" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="C29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G29" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1321,39 +1351,91 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="110">
+  <mergeCells count="114">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -1368,90 +1450,53 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{9261528D-4333-4409-BEC6-1CC0064F12C8}"/>
-    <hyperlink ref="G19" r:id="rId2" xr:uid="{709F170B-B6EA-472A-A53F-7AF1DA64CA86}"/>
-    <hyperlink ref="G18" r:id="rId3" xr:uid="{B33CA942-1C63-45CE-B54F-7F8D6A47BA95}"/>
-    <hyperlink ref="G16" r:id="rId4" xr:uid="{E2F01214-0692-4C2B-B219-82D0BF531D16}"/>
-    <hyperlink ref="G17" r:id="rId5" xr:uid="{90C71A44-4BA1-4972-974B-92B1612529B6}"/>
+    <hyperlink ref="G20" r:id="rId2" xr:uid="{709F170B-B6EA-472A-A53F-7AF1DA64CA86}"/>
+    <hyperlink ref="G19" r:id="rId3" xr:uid="{B33CA942-1C63-45CE-B54F-7F8D6A47BA95}"/>
+    <hyperlink ref="G17" r:id="rId4" xr:uid="{E2F01214-0692-4C2B-B219-82D0BF531D16}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{90C71A44-4BA1-4972-974B-92B1612529B6}"/>
     <hyperlink ref="G15" r:id="rId6" xr:uid="{524E58BE-8A02-43D4-A569-ABD1E232EE42}"/>
-    <hyperlink ref="G20" r:id="rId7" xr:uid="{A18FA11E-D65A-4714-845F-D144E2FC1382}"/>
-    <hyperlink ref="G21" r:id="rId8" xr:uid="{220FD5FF-AAC7-494B-B9E2-3DEA3AFD5A97}"/>
-    <hyperlink ref="G23" r:id="rId9" xr:uid="{E52369FE-06F1-46B5-83CA-3F819083DC7F}"/>
+    <hyperlink ref="G21" r:id="rId7" xr:uid="{A18FA11E-D65A-4714-845F-D144E2FC1382}"/>
+    <hyperlink ref="G22" r:id="rId8" xr:uid="{220FD5FF-AAC7-494B-B9E2-3DEA3AFD5A97}"/>
+    <hyperlink ref="G24" r:id="rId9" xr:uid="{E52369FE-06F1-46B5-83CA-3F819083DC7F}"/>
     <hyperlink ref="G14" r:id="rId10" xr:uid="{53BC3518-9AC4-48F1-A050-893104B9FEBD}"/>
-    <hyperlink ref="G22" r:id="rId11" xr:uid="{770FE41E-CFC3-4C0D-AAA7-85C72859D70A}"/>
+    <hyperlink ref="G23" r:id="rId11" xr:uid="{770FE41E-CFC3-4C0D-AAA7-85C72859D70A}"/>
     <hyperlink ref="G13" r:id="rId12" xr:uid="{393BAEBD-2BA3-4438-A438-08B744ABB411}"/>
-    <hyperlink ref="G27" r:id="rId13" xr:uid="{51514511-80E4-4958-BEB4-E72035065C96}"/>
-    <hyperlink ref="G26" r:id="rId14" xr:uid="{08941B07-5AB6-401A-BEB5-CFBDE5503F5D}"/>
-    <hyperlink ref="G28" r:id="rId15" xr:uid="{F7B9199A-AE3A-4F6C-AEDA-1F3C7857956F}"/>
+    <hyperlink ref="G28" r:id="rId13" xr:uid="{51514511-80E4-4958-BEB4-E72035065C96}"/>
+    <hyperlink ref="G27" r:id="rId14" xr:uid="{08941B07-5AB6-401A-BEB5-CFBDE5503F5D}"/>
+    <hyperlink ref="G29" r:id="rId15" xr:uid="{F7B9199A-AE3A-4F6C-AEDA-1F3C7857956F}"/>
+    <hyperlink ref="G16" r:id="rId16" xr:uid="{001CF274-75CF-412C-9247-FA7E13119919}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>